<commit_message>
Modifiche numero tentativi ed esportazione refusi
</commit_message>
<xml_diff>
--- a/Lista scansioni.xlsx
+++ b/Lista scansioni.xlsx
@@ -448,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>071811408270322110</t>
+          <t>071811394660722110</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A_-1A_01.jpg</t>
+          <t>WhatsApp_Image_2024-09-05_at_10.20.17.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>